<commit_message>
Yay it finally started working!!!
</commit_message>
<xml_diff>
--- a/Mappe1.xlsx
+++ b/Mappe1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fwohlgem/Documents/coding/Bingo-Card-Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75E37532-8A13-7D4B-B223-94DCCE310278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01420BDF-B4F3-3E4A-AFEA-D6B7E8FE3BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3900" yWindow="-17900" windowWidth="24940" windowHeight="15120" xr2:uid="{220BA7D0-A06C-D647-BDC5-6A71628E7791}"/>
+    <workbookView xWindow="460" yWindow="680" windowWidth="24940" windowHeight="15120" xr2:uid="{220BA7D0-A06C-D647-BDC5-6A71628E7791}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>Zelle C1</t>
   </si>
   <si>
-    <t>Zelle D1</t>
-  </si>
-  <si>
     <t>Zelle E1</t>
   </si>
   <si>
@@ -138,13 +135,16 @@
   </si>
   <si>
     <t>Zelle E5</t>
+  </si>
+  <si>
+    <t>fjdskal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +158,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -167,7 +174,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -191,15 +198,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -207,19 +223,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,26 +572,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8892E8-EEDC-AD44-A258-4BAA8504F0DD}">
-  <dimension ref="B2:J19"/>
+  <dimension ref="A2:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="2.33203125" customWidth="1"/>
-    <col min="5" max="5" width="2.1640625" customWidth="1"/>
-    <col min="7" max="7" width="2.1640625" customWidth="1"/>
-    <col min="9" max="9" width="2.1640625" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="1.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7.5" customWidth="1"/>
+    <col min="5" max="5" width="1.1640625" customWidth="1"/>
+    <col min="6" max="6" width="7.5" customWidth="1"/>
+    <col min="7" max="7" width="1.1640625" customWidth="1"/>
+    <col min="8" max="8" width="7.5" customWidth="1"/>
+    <col min="9" max="9" width="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -584,7 +607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -594,7 +617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -602,7 +625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -610,7 +633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -618,7 +641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -626,129 +649,191 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+      <c r="E10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="2:10" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="4"/>
+      <c r="F13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" s="4"/>
+      <c r="H13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" s="4"/>
+      <c r="J13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J13" t="s">
+    </row>
+    <row r="14" spans="1:13" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" s="4"/>
+      <c r="H15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" s="4"/>
+      <c r="J15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J15" t="s">
+    </row>
+    <row r="16" spans="1:13" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="6"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="4"/>
+      <c r="F17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" s="4"/>
+      <c r="H17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" s="4"/>
+      <c r="J17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J17" t="s">
+    </row>
+    <row r="18" spans="1:11" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="4"/>
+      <c r="F19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" s="4"/>
+      <c r="H19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" s="4"/>
+      <c r="J19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J19" t="s">
-        <v>33</v>
-      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C21" s="1"/>
+      <c r="E21" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>